<commit_message>
TeacherTable Index and get with Index
</commit_message>
<xml_diff>
--- a/documents/StudentManagementUsed.xlsx
+++ b/documents/StudentManagementUsed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Desktop\Student Management\StudentManagement\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274D3D7B-79CC-49F6-98F9-C175736CECC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03F349D-7137-4EEF-A85A-B4CB2A3AD7B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE44D882-7DA9-4510-BBEA-0BA7BB0D683F}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Öğrenci Tablosunda non clustered not unique index, Fakülte tablosunda nonclustered unique index kullanımı vardır</t>
-  </si>
-  <si>
     <t>View</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>Öğrenci Tablosunda insert olduğunda tetikleyip Kayıt Tarihini giren ve Öğretmen tablosunda satır silinince onu başka tabloya yazan triggerler vardır</t>
+  </si>
+  <si>
+    <t>Öğrenci Tablosunda non clustered not unique index, Fakülte tablosunda nonclustered unique index kullanımı vardır. Ogretmen tablosunda da vardir.</t>
   </si>
 </sst>
 </file>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E6015C-4660-4DBB-8983-621F2B5062AF}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -691,31 +691,31 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
         <v>34</v>
-      </c>
-      <c r="C23" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
         <v>42</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>